<commit_message>
Removed unneeded docstring whitespace. Refactored general exception handling. Refactored some language errors. Added InconsistentLanguageException. Added language_template; WIP.
</commit_message>
<xml_diff>
--- a/test/files/exceptions/language/ambiguous-default-language.xlsx
+++ b/test/files/exceptions/language/ambiguous-default-language.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51060" windowHeight="26500" tabRatio="443" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51060" windowHeight="26500" tabRatio="443"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7516" uniqueCount="2430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7782" uniqueCount="2429">
   <si>
     <t>type</t>
   </si>
@@ -7937,9 +7937,6 @@
   </si>
   <si>
     <t>ppp_input::English</t>
-  </si>
-  <si>
-    <t>label::Huh?</t>
   </si>
   <si>
     <t>#default_language</t>
@@ -8167,7 +8164,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1087">
+  <cellStyleXfs count="1091">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9259,8 +9256,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9480,8 +9481,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1087">
+  <cellStyles count="1091">
     <cellStyle name="20% - Accent6" xfId="816" builtinId="50"/>
     <cellStyle name="Excel Built-in Normal" xfId="228"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -10025,6 +10029,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1082" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1084" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1086" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1088" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1090" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -10566,6 +10572,8 @@
     <cellStyle name="Hyperlink" xfId="1081" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1083" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1085" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1087" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1089" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="37"/>
     <cellStyle name="Normal 5" xfId="231"/>
@@ -10891,11 +10899,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IY373"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="BJ1" sqref="BJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -11077,7 +11085,7 @@
         <v>2252</v>
       </c>
       <c r="AX1" s="66" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="AY1" s="66" t="s">
         <v>2411</v>
@@ -11112,9 +11120,7 @@
       <c r="BJ1" s="40" t="s">
         <v>2422</v>
       </c>
-      <c r="BK1" s="58" t="s">
-        <v>2424</v>
-      </c>
+      <c r="BK1" s="16"/>
     </row>
     <row r="2" spans="1:63" ht="13" customHeight="1">
       <c r="A2" s="40" t="s">
@@ -11124,7 +11130,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="74" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -11158,7 +11164,7 @@
       <c r="AV2" s="16"/>
       <c r="AW2" s="16"/>
       <c r="AX2" s="66" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="BA2" s="67"/>
       <c r="BB2" s="67"/>
@@ -35890,13 +35896,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U281"/>
+  <dimension ref="A1:V281"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -35905,19 +35911,19 @@
     <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" customWidth="1"/>
-    <col min="7" max="8" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="41.83203125" customWidth="1"/>
+    <col min="8" max="9" width="37.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" customHeight="1">
+    <row r="1" spans="1:13" ht="13" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>371</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
+      <c r="C1" s="76" t="s">
+        <v>327</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>1100</v>
@@ -35925,29 +35931,32 @@
       <c r="E1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="75" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>1191</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>1192</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>1193</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>1194</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>1195</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>1196</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>1197</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="13" customHeight="1">
+    <row r="2" spans="1:13" ht="13" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>372</v>
       </c>
@@ -35982,8 +35991,11 @@
       <c r="L2" s="13" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="13" customHeight="1">
+      <c r="M2" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="13" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>375</v>
       </c>
@@ -36018,8 +36030,11 @@
       <c r="L3" s="13" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="13" customHeight="1">
+      <c r="M3" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="13" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>375</v>
       </c>
@@ -36054,8 +36069,11 @@
       <c r="L4" s="13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="13" customHeight="1">
+      <c r="M4" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="13" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>379</v>
       </c>
@@ -36090,8 +36108,11 @@
       <c r="L5" s="13" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="13" customHeight="1">
+      <c r="M5" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="13" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>379</v>
       </c>
@@ -36126,8 +36147,11 @@
       <c r="L6" s="13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="13" customHeight="1">
+      <c r="M6" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>379</v>
       </c>
@@ -36162,8 +36186,11 @@
       <c r="L7" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="13" customHeight="1">
+      <c r="M7" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>381</v>
       </c>
@@ -36198,8 +36225,11 @@
       <c r="L8" s="13" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="13" customHeight="1">
+      <c r="M8" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>381</v>
       </c>
@@ -36234,8 +36264,11 @@
       <c r="L9" s="13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="13" customHeight="1">
+      <c r="M9" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>381</v>
       </c>
@@ -36270,8 +36303,11 @@
       <c r="L10" s="13" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="13" customHeight="1">
+      <c r="M10" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>381</v>
       </c>
@@ -36306,8 +36342,11 @@
       <c r="L11" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="13" customHeight="1">
+      <c r="M11" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>383</v>
       </c>
@@ -36342,8 +36381,11 @@
       <c r="L12" s="13" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="13" customHeight="1">
+      <c r="M12" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>383</v>
       </c>
@@ -36378,8 +36420,11 @@
       <c r="L13" s="13" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="13" customHeight="1">
+      <c r="M13" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>383</v>
       </c>
@@ -36414,8 +36459,11 @@
       <c r="L14" s="13" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="13" customHeight="1">
+      <c r="M14" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>383</v>
       </c>
@@ -36450,8 +36498,11 @@
       <c r="L15" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="13" customHeight="1">
+      <c r="M15" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>385</v>
       </c>
@@ -36486,8 +36537,11 @@
       <c r="L16" s="13" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="13" customHeight="1">
+      <c r="M16" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>385</v>
       </c>
@@ -36522,8 +36576,11 @@
       <c r="L17" s="13" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="13" customHeight="1">
+      <c r="M17" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="13" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>385</v>
       </c>
@@ -36558,8 +36615,11 @@
       <c r="L18" s="13" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="13" customHeight="1">
+      <c r="M18" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="13" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>385</v>
       </c>
@@ -36594,8 +36654,11 @@
       <c r="L19" s="13" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="13" customHeight="1">
+      <c r="M19" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="13" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>394</v>
       </c>
@@ -36630,8 +36693,11 @@
       <c r="L20" s="13" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="13" customHeight="1">
+      <c r="M20" s="13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>394</v>
       </c>
@@ -36666,8 +36732,11 @@
       <c r="L21" s="13" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="13" customHeight="1">
+      <c r="M21" s="13" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>394</v>
       </c>
@@ -36702,8 +36771,11 @@
       <c r="L22" s="13" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="13" customHeight="1">
+      <c r="M22" s="13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="13" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>398</v>
       </c>
@@ -36720,8 +36792,9 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A24" s="13" t="s">
         <v>399</v>
       </c>
@@ -36755,8 +36828,11 @@
       <c r="L24" s="13" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M24" s="13" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A25" s="13" t="s">
         <v>399</v>
       </c>
@@ -36790,8 +36866,11 @@
       <c r="L25" s="13" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M25" s="13" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A26" s="13" t="s">
         <v>399</v>
       </c>
@@ -36825,8 +36904,11 @@
       <c r="L26" s="13" t="s">
         <v>1182</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M26" s="13" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A27" s="13" t="s">
         <v>399</v>
       </c>
@@ -36860,8 +36942,11 @@
       <c r="L27" s="13" t="s">
         <v>1184</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M27" s="13" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A28" s="13" t="s">
         <v>399</v>
       </c>
@@ -36895,8 +36980,11 @@
       <c r="L28" s="13" t="s">
         <v>1189</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M28" s="13" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A29" s="13" t="s">
         <v>399</v>
       </c>
@@ -36930,8 +37018,11 @@
       <c r="L29" s="13" t="s">
         <v>1187</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M29" s="13" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A30" s="13" t="s">
         <v>399</v>
       </c>
@@ -36965,8 +37056,11 @@
       <c r="L30" s="13" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
+      <c r="M30" s="13" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="13" customFormat="1" ht="13" customHeight="1">
       <c r="A31" s="13" t="s">
         <v>399</v>
       </c>
@@ -37000,8 +37094,11 @@
       <c r="L31" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="13" customHeight="1">
+      <c r="M31" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="13" customHeight="1">
       <c r="A32" s="13" t="s">
         <v>401</v>
       </c>
@@ -37036,8 +37133,11 @@
       <c r="L32" s="13" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="13" customHeight="1">
+      <c r="M32" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="13" customHeight="1">
       <c r="A33" s="13" t="s">
         <v>401</v>
       </c>
@@ -37072,8 +37172,11 @@
       <c r="L33" s="13" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="13" customHeight="1">
+      <c r="M33" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="13" customHeight="1">
       <c r="A34" s="13" t="s">
         <v>401</v>
       </c>
@@ -37108,8 +37211,11 @@
       <c r="L34" s="13" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="13" customHeight="1">
+      <c r="M34" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="13" customHeight="1">
       <c r="A35" s="13" t="s">
         <v>401</v>
       </c>
@@ -37144,8 +37250,11 @@
       <c r="L35" s="13" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="13" customHeight="1">
+      <c r="M35" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="13" customHeight="1">
       <c r="A36" s="13" t="s">
         <v>401</v>
       </c>
@@ -37180,8 +37289,11 @@
       <c r="L36" s="13" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="13" customHeight="1">
+      <c r="M36" s="13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="13" customHeight="1">
       <c r="A37" s="13" t="s">
         <v>401</v>
       </c>
@@ -37216,8 +37328,11 @@
       <c r="L37" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="13" customHeight="1">
+      <c r="M37" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="13" customHeight="1">
       <c r="A38" s="13" t="s">
         <v>412</v>
       </c>
@@ -37252,8 +37367,11 @@
       <c r="L38" s="13" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="13" customHeight="1">
+      <c r="M38" s="13" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="13" customHeight="1">
       <c r="A39" s="13" t="s">
         <v>412</v>
       </c>
@@ -37288,8 +37406,11 @@
       <c r="L39" s="13" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="13" customHeight="1">
+      <c r="M39" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="13" customHeight="1">
       <c r="A40" s="13" t="s">
         <v>412</v>
       </c>
@@ -37324,8 +37445,11 @@
       <c r="L40" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="13" customHeight="1">
+      <c r="M40" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="13" customHeight="1">
       <c r="A41" s="13" t="s">
         <v>417</v>
       </c>
@@ -37360,8 +37484,11 @@
       <c r="L41" s="13" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="13" customHeight="1">
+      <c r="M41" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="13" customHeight="1">
       <c r="A42" s="13" t="s">
         <v>417</v>
       </c>
@@ -37396,8 +37523,11 @@
       <c r="L42" s="13" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="13" customHeight="1">
+      <c r="M42" s="13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="13" customHeight="1">
       <c r="A43" s="13" t="s">
         <v>417</v>
       </c>
@@ -37432,8 +37562,11 @@
       <c r="L43" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="13" customHeight="1">
+      <c r="M43" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="13" customHeight="1">
       <c r="A44" s="13" t="s">
         <v>422</v>
       </c>
@@ -37468,8 +37601,11 @@
       <c r="L44" s="13" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="13" customHeight="1">
+      <c r="M44" s="13" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="13" customHeight="1">
       <c r="A45" s="13" t="s">
         <v>422</v>
       </c>
@@ -37504,8 +37640,11 @@
       <c r="L45" s="13" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="13" customHeight="1">
+      <c r="M45" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="13" customHeight="1">
       <c r="A46" s="13" t="s">
         <v>422</v>
       </c>
@@ -37540,8 +37679,11 @@
       <c r="L46" s="13" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="13" customHeight="1">
+      <c r="M46" s="13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="13" customHeight="1">
       <c r="A47" s="13" t="s">
         <v>422</v>
       </c>
@@ -37576,8 +37718,11 @@
       <c r="L47" s="13" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="13" customHeight="1">
+      <c r="M47" s="13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="13" customHeight="1">
       <c r="A48" s="13" t="s">
         <v>422</v>
       </c>
@@ -37612,8 +37757,11 @@
       <c r="L48" s="13" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="13" customHeight="1">
+      <c r="M48" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="13" customHeight="1">
       <c r="A49" s="13" t="s">
         <v>422</v>
       </c>
@@ -37648,8 +37796,11 @@
       <c r="L49" s="13" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="13" customHeight="1">
+      <c r="M49" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="13" customHeight="1">
       <c r="A50" s="13" t="s">
         <v>422</v>
       </c>
@@ -37684,8 +37835,11 @@
       <c r="L50" s="13" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="13" customHeight="1">
+      <c r="M50" s="13" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="13" customHeight="1">
       <c r="A51" s="13" t="s">
         <v>422</v>
       </c>
@@ -37720,8 +37874,11 @@
       <c r="L51" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M51" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A52" s="15" t="s">
         <v>842</v>
       </c>
@@ -37756,8 +37913,11 @@
       <c r="L52" s="15" t="s">
         <v>843</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M52" s="15" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>842</v>
       </c>
@@ -37792,8 +37952,11 @@
       <c r="L53" s="15" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M53" s="15" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>842</v>
       </c>
@@ -37828,8 +37991,11 @@
       <c r="L54" s="15" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M54" s="15" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A55" s="15" t="s">
         <v>842</v>
       </c>
@@ -37864,8 +38030,11 @@
       <c r="L55" s="15" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M55" s="15" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A56" s="15" t="s">
         <v>842</v>
       </c>
@@ -37900,8 +38069,11 @@
       <c r="L56" s="15" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M56" s="15" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A57" s="15" t="s">
         <v>847</v>
       </c>
@@ -37936,8 +38108,11 @@
       <c r="L57" s="15" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M57" s="15" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A58" s="15" t="s">
         <v>847</v>
       </c>
@@ -37972,8 +38147,11 @@
       <c r="L58" s="15" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M58" s="15" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A59" s="15" t="s">
         <v>847</v>
       </c>
@@ -38008,8 +38186,11 @@
       <c r="L59" s="15" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M59" s="15" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A60" s="15" t="s">
         <v>847</v>
       </c>
@@ -38044,8 +38225,11 @@
       <c r="L60" s="15" t="s">
         <v>846</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
+      <c r="M60" s="15" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A61" s="15" t="s">
         <v>847</v>
       </c>
@@ -38080,8 +38264,11 @@
       <c r="L61" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="13" customHeight="1">
+      <c r="M61" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="13" customHeight="1">
       <c r="A62" s="13" t="s">
         <v>440</v>
       </c>
@@ -38116,8 +38303,11 @@
       <c r="L62" s="13" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="13" customHeight="1">
+      <c r="M62" s="13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="13" customHeight="1">
       <c r="A63" s="13" t="s">
         <v>440</v>
       </c>
@@ -38152,8 +38342,11 @@
       <c r="L63" s="13" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="13" customHeight="1">
+      <c r="M63" s="13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="13" customHeight="1">
       <c r="A64" s="13" t="s">
         <v>440</v>
       </c>
@@ -38188,8 +38381,11 @@
       <c r="L64" s="13" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" ht="13" customHeight="1">
+      <c r="M64" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="13" customHeight="1">
       <c r="A65" s="13" t="s">
         <v>440</v>
       </c>
@@ -38224,8 +38420,11 @@
       <c r="L65" s="13" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="13" customHeight="1">
+      <c r="M65" s="13" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="13" customHeight="1">
       <c r="A66" s="13" t="s">
         <v>440</v>
       </c>
@@ -38260,8 +38459,11 @@
       <c r="L66" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" ht="13" customHeight="1">
+      <c r="M66" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="13" customHeight="1">
       <c r="A67" s="13" t="s">
         <v>440</v>
       </c>
@@ -38296,8 +38498,11 @@
       <c r="L67" s="13" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="13" customHeight="1">
+      <c r="M67" s="13" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="13" customHeight="1">
       <c r="A68" s="13" t="s">
         <v>440</v>
       </c>
@@ -38332,8 +38537,11 @@
       <c r="L68" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="13" customHeight="1">
+      <c r="M68" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="13" customHeight="1">
       <c r="A69" s="13" t="s">
         <v>448</v>
       </c>
@@ -38368,8 +38576,11 @@
       <c r="L69" s="13" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="13" customHeight="1">
+      <c r="M69" s="13" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="13" customHeight="1">
       <c r="A70" s="13" t="s">
         <v>448</v>
       </c>
@@ -38404,8 +38615,11 @@
       <c r="L70" s="13" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" ht="13" customHeight="1">
+      <c r="M70" s="13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="13" customHeight="1">
       <c r="A71" s="13" t="s">
         <v>448</v>
       </c>
@@ -38440,8 +38654,11 @@
       <c r="L71" s="13" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" ht="13" customHeight="1">
+      <c r="M71" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="13" customHeight="1">
       <c r="A72" s="13" t="s">
         <v>448</v>
       </c>
@@ -38476,8 +38693,11 @@
       <c r="L72" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" s="5" customFormat="1" ht="13" customHeight="1">
+      <c r="M72" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>455</v>
       </c>
@@ -38512,8 +38732,11 @@
       <c r="L73" s="13" t="s">
         <v>1753</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M73" s="13" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>455</v>
       </c>
@@ -38548,8 +38771,11 @@
       <c r="L74" s="13" t="s">
         <v>1754</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M74" s="13" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>455</v>
       </c>
@@ -38584,8 +38810,11 @@
       <c r="L75" s="13" t="s">
         <v>1755</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M75" s="13" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>455</v>
       </c>
@@ -38620,8 +38849,11 @@
       <c r="L76" s="13" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M76" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>455</v>
       </c>
@@ -38656,8 +38888,11 @@
       <c r="L77" s="13" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M77" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>455</v>
       </c>
@@ -38692,8 +38927,11 @@
       <c r="L78" s="13" t="s">
         <v>1756</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M78" s="13" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>455</v>
       </c>
@@ -38728,8 +38966,11 @@
       <c r="L79" s="13" t="s">
         <v>1757</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M79" s="13" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>455</v>
       </c>
@@ -38764,8 +39005,11 @@
       <c r="L80" s="13" t="s">
         <v>1758</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M80" s="13" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>455</v>
       </c>
@@ -38800,8 +39044,11 @@
       <c r="L81" s="13" t="s">
         <v>1759</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M81" s="13" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>455</v>
       </c>
@@ -38836,8 +39083,11 @@
       <c r="L82" s="13" t="s">
         <v>1760</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M82" s="13" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>455</v>
       </c>
@@ -38872,8 +39122,11 @@
       <c r="L83" s="13" t="s">
         <v>1761</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M83" s="13" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>455</v>
       </c>
@@ -38908,8 +39161,11 @@
       <c r="L84" s="13" t="s">
         <v>1762</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M84" s="13" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>455</v>
       </c>
@@ -38944,8 +39200,11 @@
       <c r="L85" s="13" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M85" s="13" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>455</v>
       </c>
@@ -38980,8 +39239,11 @@
       <c r="L86" s="13" t="s">
         <v>1763</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M86" s="13" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>455</v>
       </c>
@@ -39016,8 +39278,11 @@
       <c r="L87" s="13" t="s">
         <v>1764</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M87" s="13" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>455</v>
       </c>
@@ -39052,8 +39317,11 @@
       <c r="L88" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M88" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>580</v>
       </c>
@@ -39088,8 +39356,11 @@
       <c r="L89" s="13" t="s">
         <v>1755</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M89" s="13" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>580</v>
       </c>
@@ -39124,8 +39395,11 @@
       <c r="L90" s="13" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M90" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>580</v>
       </c>
@@ -39160,8 +39434,11 @@
       <c r="L91" s="13" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M91" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>580</v>
       </c>
@@ -39196,8 +39473,11 @@
       <c r="L92" s="13" t="s">
         <v>1756</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M92" s="13" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>580</v>
       </c>
@@ -39232,8 +39512,11 @@
       <c r="L93" s="13" t="s">
         <v>1757</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M93" s="13" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>580</v>
       </c>
@@ -39268,8 +39551,11 @@
       <c r="L94" s="13" t="s">
         <v>1758</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M94" s="13" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>580</v>
       </c>
@@ -39304,8 +39590,11 @@
       <c r="L95" s="13" t="s">
         <v>1759</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M95" s="13" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>580</v>
       </c>
@@ -39340,8 +39629,11 @@
       <c r="L96" s="13" t="s">
         <v>1760</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M96" s="13" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>580</v>
       </c>
@@ -39376,8 +39668,11 @@
       <c r="L97" s="13" t="s">
         <v>1761</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M97" s="13" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>580</v>
       </c>
@@ -39412,8 +39707,11 @@
       <c r="L98" s="13" t="s">
         <v>1762</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M98" s="13" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>580</v>
       </c>
@@ -39448,8 +39746,11 @@
       <c r="L99" s="13" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M99" s="13" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>580</v>
       </c>
@@ -39484,8 +39785,11 @@
       <c r="L100" s="13" t="s">
         <v>1763</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M100" s="13" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>580</v>
       </c>
@@ -39520,8 +39824,11 @@
       <c r="L101" s="13" t="s">
         <v>1764</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M101" s="13" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>580</v>
       </c>
@@ -39556,8 +39863,11 @@
       <c r="L102" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" ht="13" customHeight="1">
+      <c r="M102" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="13" customHeight="1">
       <c r="A103" s="13" t="s">
         <v>483</v>
       </c>
@@ -39592,8 +39902,11 @@
       <c r="L103" s="13" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" ht="13" customHeight="1">
+      <c r="M103" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="13" customHeight="1">
       <c r="A104" s="13" t="s">
         <v>483</v>
       </c>
@@ -39628,8 +39941,11 @@
       <c r="L104" s="13" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" ht="13" customHeight="1">
+      <c r="M104" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="13" customHeight="1">
       <c r="A105" s="13" t="s">
         <v>483</v>
       </c>
@@ -39664,8 +39980,11 @@
       <c r="L105" s="13" t="s">
         <v>1765</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" ht="13" customHeight="1">
+      <c r="M105" s="13" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="13" customHeight="1">
       <c r="A106" s="13" t="s">
         <v>483</v>
       </c>
@@ -39700,8 +40019,11 @@
       <c r="L106" s="13" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" ht="13" customHeight="1">
+      <c r="M106" s="13" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="13" customHeight="1">
       <c r="A107" s="13" t="s">
         <v>483</v>
       </c>
@@ -39736,8 +40058,11 @@
       <c r="L107" s="13" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" ht="13" customHeight="1">
+      <c r="M107" s="13" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="13" customHeight="1">
       <c r="A108" s="13" t="s">
         <v>483</v>
       </c>
@@ -39772,8 +40097,11 @@
       <c r="L108" s="13" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" ht="13" customHeight="1">
+      <c r="M108" s="13" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="13" customHeight="1">
       <c r="A109" s="13" t="s">
         <v>483</v>
       </c>
@@ -39808,8 +40136,11 @@
       <c r="L109" s="13" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" ht="13" customHeight="1">
+      <c r="M109" s="13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="13" customHeight="1">
       <c r="A110" s="13" t="s">
         <v>483</v>
       </c>
@@ -39844,8 +40175,11 @@
       <c r="L110" s="13" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" ht="13" customHeight="1">
+      <c r="M110" s="13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="13" customHeight="1">
       <c r="A111" s="13" t="s">
         <v>483</v>
       </c>
@@ -39880,8 +40214,11 @@
       <c r="L111" s="13" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" ht="13" customHeight="1">
+      <c r="M111" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="13" customHeight="1">
       <c r="A112" s="13" t="s">
         <v>483</v>
       </c>
@@ -39916,8 +40253,11 @@
       <c r="L112" s="13" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" ht="13" customHeight="1">
+      <c r="M112" s="13" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="13" customHeight="1">
       <c r="A113" s="13" t="s">
         <v>483</v>
       </c>
@@ -39952,8 +40292,11 @@
       <c r="L113" s="13" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" ht="13" customHeight="1">
+      <c r="M113" s="13" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="13" customHeight="1">
       <c r="A114" s="13" t="s">
         <v>483</v>
       </c>
@@ -39988,8 +40331,11 @@
       <c r="L114" s="13" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" ht="13" customHeight="1">
+      <c r="M114" s="13" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="13" customHeight="1">
       <c r="A115" s="13" t="s">
         <v>483</v>
       </c>
@@ -40024,8 +40370,11 @@
       <c r="L115" s="13" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" ht="13" customHeight="1">
+      <c r="M115" s="13" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="13" customHeight="1">
       <c r="A116" s="13" t="s">
         <v>483</v>
       </c>
@@ -40060,8 +40409,11 @@
       <c r="L116" s="13" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" ht="13" customHeight="1">
+      <c r="M116" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="13" customHeight="1">
       <c r="A117" s="13" t="s">
         <v>483</v>
       </c>
@@ -40096,8 +40448,11 @@
       <c r="L117" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" ht="13" customHeight="1">
+      <c r="M117" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="13" customHeight="1">
       <c r="A118" s="13" t="s">
         <v>483</v>
       </c>
@@ -40132,8 +40487,11 @@
       <c r="L118" s="13" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" ht="13" customHeight="1">
+      <c r="M118" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="13" customHeight="1">
       <c r="A119" s="13" t="s">
         <v>483</v>
       </c>
@@ -40168,8 +40526,11 @@
       <c r="L119" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" ht="13" customHeight="1">
+      <c r="M119" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="13" customHeight="1">
       <c r="A120" s="13" t="s">
         <v>512</v>
       </c>
@@ -40204,8 +40565,11 @@
       <c r="L120" s="13" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" ht="13" customHeight="1">
+      <c r="M120" s="13" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="13" customHeight="1">
       <c r="A121" s="13" t="s">
         <v>512</v>
       </c>
@@ -40240,8 +40604,11 @@
       <c r="L121" s="13" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" ht="13" customHeight="1">
+      <c r="M121" s="13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="13" customHeight="1">
       <c r="A122" s="13" t="s">
         <v>512</v>
       </c>
@@ -40276,8 +40643,11 @@
       <c r="L122" s="13" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" ht="13" customHeight="1">
+      <c r="M122" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="13" customHeight="1">
       <c r="A123" s="13" t="s">
         <v>512</v>
       </c>
@@ -40312,8 +40682,11 @@
       <c r="L123" s="13" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" ht="13" customHeight="1">
+      <c r="M123" s="13" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="13" customHeight="1">
       <c r="A124" s="13" t="s">
         <v>512</v>
       </c>
@@ -40348,8 +40721,11 @@
       <c r="L124" s="13" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" ht="13" customHeight="1">
+      <c r="M124" s="13" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="13" customHeight="1">
       <c r="A125" s="13" t="s">
         <v>512</v>
       </c>
@@ -40384,8 +40760,11 @@
       <c r="L125" s="13" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" ht="13" customHeight="1">
+      <c r="M125" s="13" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="13" customHeight="1">
       <c r="A126" s="13" t="s">
         <v>512</v>
       </c>
@@ -40420,8 +40799,11 @@
       <c r="L126" s="13" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" ht="13" customHeight="1">
+      <c r="M126" s="13" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="13" customHeight="1">
       <c r="A127" s="13" t="s">
         <v>512</v>
       </c>
@@ -40456,8 +40838,11 @@
       <c r="L127" s="13" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" ht="13" customHeight="1">
+      <c r="M127" s="13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="13" customHeight="1">
       <c r="A128" s="13" t="s">
         <v>512</v>
       </c>
@@ -40492,8 +40877,11 @@
       <c r="L128" s="13" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" ht="13" customHeight="1">
+      <c r="M128" s="13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="13" customHeight="1">
       <c r="A129" s="13" t="s">
         <v>512</v>
       </c>
@@ -40528,8 +40916,11 @@
       <c r="L129" s="13" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" ht="13" customHeight="1">
+      <c r="M129" s="13" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="13" customHeight="1">
       <c r="A130" s="13" t="s">
         <v>512</v>
       </c>
@@ -40564,8 +40955,11 @@
       <c r="L130" s="13" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" ht="13" customHeight="1">
+      <c r="M130" s="13" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="13" customHeight="1">
       <c r="A131" s="13" t="s">
         <v>512</v>
       </c>
@@ -40600,8 +40994,11 @@
       <c r="L131" s="13" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" ht="13" customHeight="1">
+      <c r="M131" s="13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="13" customHeight="1">
       <c r="A132" s="13" t="s">
         <v>512</v>
       </c>
@@ -40636,8 +41033,11 @@
       <c r="L132" s="13" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" ht="13" customHeight="1">
+      <c r="M132" s="13" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="13" customHeight="1">
       <c r="A133" s="13" t="s">
         <v>512</v>
       </c>
@@ -40672,8 +41072,11 @@
       <c r="L133" s="13" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" ht="13" customHeight="1">
+      <c r="M133" s="13" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="13" customHeight="1">
       <c r="A134" s="13" t="s">
         <v>512</v>
       </c>
@@ -40708,8 +41111,11 @@
       <c r="L134" s="13" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" ht="13" customHeight="1">
+      <c r="M134" s="13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="13" customHeight="1">
       <c r="A135" s="13" t="s">
         <v>512</v>
       </c>
@@ -40744,8 +41150,11 @@
       <c r="L135" s="13" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" ht="13" customHeight="1">
+      <c r="M135" s="13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="13" customHeight="1">
       <c r="A136" s="13" t="s">
         <v>512</v>
       </c>
@@ -40780,8 +41189,11 @@
       <c r="L136" s="13" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" ht="13" customHeight="1">
+      <c r="M136" s="13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="13" customHeight="1">
       <c r="A137" s="13" t="s">
         <v>512</v>
       </c>
@@ -40816,8 +41228,11 @@
       <c r="L137" s="13" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" ht="13" customHeight="1">
+      <c r="M137" s="13" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="13" customHeight="1">
       <c r="A138" s="13" t="s">
         <v>512</v>
       </c>
@@ -40852,8 +41267,11 @@
       <c r="L138" s="13" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" ht="13" customHeight="1">
+      <c r="M138" s="13" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="13" customHeight="1">
       <c r="A139" s="13" t="s">
         <v>512</v>
       </c>
@@ -40888,8 +41306,11 @@
       <c r="L139" s="13" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" ht="13" customHeight="1">
+      <c r="M139" s="13" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="13" customHeight="1">
       <c r="A140" s="13" t="s">
         <v>512</v>
       </c>
@@ -40924,8 +41345,11 @@
       <c r="L140" s="13" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" ht="13" customHeight="1">
+      <c r="M140" s="13" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="13" customHeight="1">
       <c r="A141" s="13" t="s">
         <v>512</v>
       </c>
@@ -40960,8 +41384,11 @@
       <c r="L141" s="13" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" ht="13" customHeight="1">
+      <c r="M141" s="13" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="13" customHeight="1">
       <c r="A142" s="13" t="s">
         <v>512</v>
       </c>
@@ -40996,8 +41423,11 @@
       <c r="L142" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" ht="13" customHeight="1">
+      <c r="M142" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="13" customHeight="1">
       <c r="A143" s="13" t="s">
         <v>512</v>
       </c>
@@ -41032,8 +41462,11 @@
       <c r="L143" s="13" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" ht="13" customHeight="1">
+      <c r="M143" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="13" customHeight="1">
       <c r="A144" s="13" t="s">
         <v>512</v>
       </c>
@@ -41068,8 +41501,11 @@
       <c r="L144" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" ht="13" customHeight="1">
+      <c r="M144" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" ht="13" customHeight="1">
       <c r="A145" s="13" t="s">
         <v>543</v>
       </c>
@@ -41104,8 +41540,11 @@
       <c r="L145" s="13" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" ht="13" customHeight="1">
+      <c r="M145" s="13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="13" customHeight="1">
       <c r="A146" s="13" t="s">
         <v>543</v>
       </c>
@@ -41140,8 +41579,11 @@
       <c r="L146" s="13" t="s">
         <v>1766</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" ht="13" customHeight="1">
+      <c r="M146" s="13" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="13" customHeight="1">
       <c r="A147" s="13" t="s">
         <v>543</v>
       </c>
@@ -41176,8 +41618,11 @@
       <c r="L147" s="13" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" ht="13" customHeight="1">
+      <c r="M147" s="13" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="13" customHeight="1">
       <c r="A148" s="13" t="s">
         <v>543</v>
       </c>
@@ -41212,8 +41657,11 @@
       <c r="L148" s="13" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" ht="13" customHeight="1">
+      <c r="M148" s="13" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="13" customHeight="1">
       <c r="A149" s="13" t="s">
         <v>543</v>
       </c>
@@ -41248,8 +41696,11 @@
       <c r="L149" s="13" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" ht="13" customHeight="1">
+      <c r="M149" s="13" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" ht="13" customHeight="1">
       <c r="A150" s="13" t="s">
         <v>543</v>
       </c>
@@ -41284,8 +41735,11 @@
       <c r="L150" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" ht="13" customHeight="1">
+      <c r="M150" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="13" customHeight="1">
       <c r="A151" s="13" t="s">
         <v>543</v>
       </c>
@@ -41320,8 +41774,11 @@
       <c r="L151" s="13" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" ht="13" customHeight="1">
+      <c r="M151" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="13" customHeight="1">
       <c r="A152" s="13" t="s">
         <v>543</v>
       </c>
@@ -41356,8 +41813,11 @@
       <c r="L152" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" ht="13" customHeight="1">
+      <c r="M152" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="13" customHeight="1">
       <c r="A153" s="13" t="s">
         <v>554</v>
       </c>
@@ -41392,8 +41852,11 @@
       <c r="L153" s="13" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" ht="13" customHeight="1">
+      <c r="M153" s="13" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="13" customHeight="1">
       <c r="A154" s="13" t="s">
         <v>554</v>
       </c>
@@ -41428,8 +41891,11 @@
       <c r="L154" s="13" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" ht="13" customHeight="1">
+      <c r="M154" s="13" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="13" customHeight="1">
       <c r="A155" s="13" t="s">
         <v>554</v>
       </c>
@@ -41464,8 +41930,11 @@
       <c r="L155" s="13" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" ht="13" customHeight="1">
+      <c r="M155" s="13" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="13" customHeight="1">
       <c r="A156" s="13" t="s">
         <v>554</v>
       </c>
@@ -41500,8 +41969,11 @@
       <c r="L156" s="13" t="s">
         <v>1119</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" ht="13" customHeight="1">
+      <c r="M156" s="13" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="13" customHeight="1">
       <c r="A157" s="13" t="s">
         <v>554</v>
       </c>
@@ -41536,8 +42008,11 @@
       <c r="L157" s="13" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" ht="13" customHeight="1">
+      <c r="M157" s="13" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="13" customHeight="1">
       <c r="A158" s="13" t="s">
         <v>554</v>
       </c>
@@ -41572,8 +42047,11 @@
       <c r="L158" s="13" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" ht="13" customHeight="1">
+      <c r="M158" s="13" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="13" customHeight="1">
       <c r="A159" s="13" t="s">
         <v>554</v>
       </c>
@@ -41608,8 +42086,11 @@
       <c r="L159" s="13" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" ht="13" customHeight="1">
+      <c r="M159" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="13" customHeight="1">
       <c r="A160" s="13" t="s">
         <v>554</v>
       </c>
@@ -41644,8 +42125,11 @@
       <c r="L160" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" ht="13" customHeight="1">
+      <c r="M160" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="13" customHeight="1">
       <c r="A161" s="13" t="s">
         <v>554</v>
       </c>
@@ -41680,8 +42164,11 @@
       <c r="L161" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" ht="13" customHeight="1">
+      <c r="M161" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="13" customHeight="1">
       <c r="A162" s="13" t="s">
         <v>566</v>
       </c>
@@ -41716,8 +42203,11 @@
       <c r="L162" s="13" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" ht="13" customHeight="1">
+      <c r="M162" s="13" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="13" customHeight="1">
       <c r="A163" s="13" t="s">
         <v>566</v>
       </c>
@@ -41752,8 +42242,11 @@
       <c r="L163" s="13" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" ht="13" customHeight="1">
+      <c r="M163" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="13" customHeight="1">
       <c r="A164" s="13" t="s">
         <v>566</v>
       </c>
@@ -41788,8 +42281,11 @@
       <c r="L164" s="13" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" ht="13" customHeight="1">
+      <c r="M164" s="13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="13" customHeight="1">
       <c r="A165" s="13" t="s">
         <v>566</v>
       </c>
@@ -41824,8 +42320,11 @@
       <c r="L165" s="13" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" ht="13" customHeight="1">
+      <c r="M165" s="13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="13" customHeight="1">
       <c r="A166" s="13" t="s">
         <v>566</v>
       </c>
@@ -41860,8 +42359,11 @@
       <c r="L166" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" ht="13" customHeight="1">
+      <c r="M166" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="13" customHeight="1">
       <c r="A167" s="13" t="s">
         <v>567</v>
       </c>
@@ -41896,8 +42398,11 @@
       <c r="L167" s="13" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" ht="13" customHeight="1">
+      <c r="M167" s="13" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="13" customHeight="1">
       <c r="A168" s="13" t="s">
         <v>567</v>
       </c>
@@ -41932,8 +42437,11 @@
       <c r="L168" s="13" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" ht="13" customHeight="1">
+      <c r="M168" s="13" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="13" customHeight="1">
       <c r="A169" s="13" t="s">
         <v>567</v>
       </c>
@@ -41968,8 +42476,11 @@
       <c r="L169" s="13" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" ht="13" customHeight="1">
+      <c r="M169" s="13" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="13" customHeight="1">
       <c r="A170" s="13" t="s">
         <v>567</v>
       </c>
@@ -42004,8 +42515,11 @@
       <c r="L170" s="13" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" ht="13" customHeight="1">
+      <c r="M170" s="13" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" ht="13" customHeight="1">
       <c r="A171" s="13" t="s">
         <v>567</v>
       </c>
@@ -42040,8 +42554,11 @@
       <c r="L171" s="13" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" ht="13" customHeight="1">
+      <c r="M171" s="13" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="13" customHeight="1">
       <c r="A172" s="13" t="s">
         <v>567</v>
       </c>
@@ -42076,8 +42593,11 @@
       <c r="L172" s="13" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" s="14" customFormat="1" ht="13" customHeight="1">
+      <c r="M172" s="13" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" s="14" customFormat="1" ht="13" customHeight="1">
       <c r="A173" s="18" t="s">
         <v>586</v>
       </c>
@@ -42112,8 +42632,11 @@
       <c r="L173" s="18" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" s="14" customFormat="1" ht="13" customHeight="1">
+      <c r="M173" s="18" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" s="14" customFormat="1" ht="13" customHeight="1">
       <c r="A174" s="18" t="s">
         <v>586</v>
       </c>
@@ -42148,8 +42671,11 @@
       <c r="L174" s="18" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" s="14" customFormat="1" ht="13" customHeight="1">
+      <c r="M174" s="18" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" s="14" customFormat="1" ht="13" customHeight="1">
       <c r="A175" s="18" t="s">
         <v>586</v>
       </c>
@@ -42184,8 +42710,11 @@
       <c r="L175" s="18" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" s="14" customFormat="1" ht="13" customHeight="1">
+      <c r="M175" s="18" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" s="14" customFormat="1" ht="13" customHeight="1">
       <c r="A176" s="18" t="s">
         <v>586</v>
       </c>
@@ -42220,8 +42749,11 @@
       <c r="L176" s="13" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M176" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A177" s="18" t="s">
         <v>594</v>
       </c>
@@ -42256,8 +42788,11 @@
       <c r="L177" s="13" t="s">
         <v>1232</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M177" s="13" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A178" s="18" t="s">
         <v>594</v>
       </c>
@@ -42292,8 +42827,11 @@
       <c r="L178" s="13" t="s">
         <v>1234</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M178" s="13" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A179" s="18" t="s">
         <v>594</v>
       </c>
@@ -42328,8 +42866,11 @@
       <c r="L179" s="13" t="s">
         <v>1236</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M179" s="13" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A180" s="18" t="s">
         <v>594</v>
       </c>
@@ -42364,8 +42905,11 @@
       <c r="L180" s="13" t="s">
         <v>1238</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M180" s="13" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A181" s="18" t="s">
         <v>594</v>
       </c>
@@ -42400,8 +42944,11 @@
       <c r="L181" s="13" t="s">
         <v>1240</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M181" s="13" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A182" s="18" t="s">
         <v>594</v>
       </c>
@@ -42436,8 +42983,11 @@
       <c r="L182" s="13" t="s">
         <v>1242</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M182" s="13" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A183" s="18" t="s">
         <v>594</v>
       </c>
@@ -42472,8 +43022,11 @@
       <c r="L183" s="13" t="s">
         <v>1244</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M183" s="13" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A184" s="18" t="s">
         <v>594</v>
       </c>
@@ -42508,8 +43061,11 @@
       <c r="L184" s="13" t="s">
         <v>1085</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M184" s="13" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A185" s="18" t="s">
         <v>594</v>
       </c>
@@ -42544,8 +43100,11 @@
       <c r="L185" s="13" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M185" s="13" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A186" s="18" t="s">
         <v>594</v>
       </c>
@@ -42580,8 +43139,11 @@
       <c r="L186" s="13" t="s">
         <v>1248</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M186" s="13" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A187" s="18" t="s">
         <v>594</v>
       </c>
@@ -42616,8 +43178,11 @@
       <c r="L187" s="13" t="s">
         <v>1250</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M187" s="13" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A188" s="18" t="s">
         <v>594</v>
       </c>
@@ -42652,8 +43217,11 @@
       <c r="L188" s="13" t="s">
         <v>1252</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M188" s="13" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A189" s="18" t="s">
         <v>594</v>
       </c>
@@ -42688,8 +43256,11 @@
       <c r="L189" s="13" t="s">
         <v>1254</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M189" s="13" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A190" s="18" t="s">
         <v>594</v>
       </c>
@@ -42724,8 +43295,11 @@
       <c r="L190" s="13" t="s">
         <v>1255</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M190" s="13" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A191" s="18" t="s">
         <v>594</v>
       </c>
@@ -42760,8 +43334,11 @@
       <c r="L191" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M191" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A192" s="18" t="s">
         <v>594</v>
       </c>
@@ -42796,8 +43373,11 @@
       <c r="L192" s="13" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M192" s="13" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A193" s="18" t="s">
         <v>594</v>
       </c>
@@ -42832,8 +43412,11 @@
       <c r="L193" s="13" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M193" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A194" s="23" t="s">
         <v>836</v>
       </c>
@@ -42868,8 +43451,11 @@
       <c r="L194" s="24" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M194" s="24" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A195" s="25" t="s">
         <v>836</v>
       </c>
@@ -42904,8 +43490,11 @@
       <c r="L195" s="3" t="s">
         <v>839</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M195" s="3" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A196" s="25" t="s">
         <v>836</v>
       </c>
@@ -42940,8 +43529,11 @@
       <c r="L196" s="3" t="s">
         <v>841</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M196" s="3" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A197" s="25" t="s">
         <v>836</v>
       </c>
@@ -42976,8 +43568,11 @@
       <c r="L197" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
+      <c r="M197" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A198" s="25" t="s">
         <v>836</v>
       </c>
@@ -43012,8 +43607,11 @@
       <c r="L198" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" s="5" customFormat="1" ht="13" customHeight="1">
+      <c r="M198" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1">
       <c r="A199" s="2" t="s">
         <v>603</v>
       </c>
@@ -43048,8 +43646,11 @@
       <c r="L199" s="4" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M199" s="4" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A200" s="6" t="s">
         <v>603</v>
       </c>
@@ -43084,8 +43685,11 @@
       <c r="L200" s="6" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M200" s="6" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A201" s="6" t="s">
         <v>603</v>
       </c>
@@ -43120,8 +43724,11 @@
       <c r="L201" s="6" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M201" s="6" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A202" s="6" t="s">
         <v>603</v>
       </c>
@@ -43156,8 +43763,11 @@
       <c r="L202" s="6" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M202" s="6" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A203" s="6" t="s">
         <v>603</v>
       </c>
@@ -43192,8 +43802,11 @@
       <c r="L203" s="6" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M203" s="6" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A204" s="6" t="s">
         <v>603</v>
       </c>
@@ -43228,8 +43841,11 @@
       <c r="L204" s="6" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M204" s="6" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A205" s="6" t="s">
         <v>603</v>
       </c>
@@ -43264,8 +43880,11 @@
       <c r="L205" s="6" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M205" s="6" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A206" s="6" t="s">
         <v>603</v>
       </c>
@@ -43300,8 +43919,11 @@
       <c r="L206" s="6" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M206" s="6" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A207" s="6" t="s">
         <v>603</v>
       </c>
@@ -43336,8 +43958,11 @@
       <c r="L207" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" s="5" customFormat="1" ht="13" customHeight="1">
+      <c r="M207" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1">
       <c r="A208" s="2" t="s">
         <v>603</v>
       </c>
@@ -43372,8 +43997,11 @@
       <c r="L208" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M208" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A209" s="6" t="s">
         <v>620</v>
       </c>
@@ -43408,8 +44036,11 @@
       <c r="L209" s="6" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M209" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A210" s="6" t="s">
         <v>620</v>
       </c>
@@ -43444,8 +44075,11 @@
       <c r="L210" s="6" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M210" s="6" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A211" s="6" t="s">
         <v>620</v>
       </c>
@@ -43480,8 +44114,11 @@
       <c r="L211" s="6" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M211" s="6" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A212" s="6" t="s">
         <v>620</v>
       </c>
@@ -43516,8 +44153,11 @@
       <c r="L212" s="6" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M212" s="6" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A213" s="6" t="s">
         <v>620</v>
       </c>
@@ -43552,8 +44192,11 @@
       <c r="L213" s="6" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M213" s="6" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A214" s="6" t="s">
         <v>620</v>
       </c>
@@ -43588,8 +44231,11 @@
       <c r="L214" s="6" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="215" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M214" s="6" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A215" s="6" t="s">
         <v>620</v>
       </c>
@@ -43624,8 +44270,11 @@
       <c r="L215" s="6" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="216" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M215" s="6" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A216" s="6" t="s">
         <v>620</v>
       </c>
@@ -43660,8 +44309,11 @@
       <c r="L216" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="217" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M216" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A217" s="6" t="s">
         <v>632</v>
       </c>
@@ -43696,8 +44348,11 @@
       <c r="L217" s="6" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="218" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M217" s="6" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A218" s="6" t="s">
         <v>632</v>
       </c>
@@ -43732,8 +44387,11 @@
       <c r="L218" s="6" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M218" s="6" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A219" s="6" t="s">
         <v>632</v>
       </c>
@@ -43768,8 +44426,11 @@
       <c r="L219" s="6" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M219" s="6" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A220" s="6" t="s">
         <v>632</v>
       </c>
@@ -43804,8 +44465,11 @@
       <c r="L220" s="6" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="221" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M220" s="6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A221" s="6" t="s">
         <v>632</v>
       </c>
@@ -43840,8 +44504,11 @@
       <c r="L221" s="6" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M221" s="6" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A222" s="6" t="s">
         <v>632</v>
       </c>
@@ -43876,8 +44543,11 @@
       <c r="L222" s="6" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M222" s="6" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A223" s="6" t="s">
         <v>632</v>
       </c>
@@ -43912,8 +44582,11 @@
       <c r="L223" s="6" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M223" s="6" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A224" s="6" t="s">
         <v>632</v>
       </c>
@@ -43948,8 +44621,11 @@
       <c r="L224" s="6" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="225" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M224" s="6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A225" s="6" t="s">
         <v>632</v>
       </c>
@@ -43984,8 +44660,11 @@
       <c r="L225" s="6" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M225" s="6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A226" s="6" t="s">
         <v>632</v>
       </c>
@@ -44020,8 +44699,11 @@
       <c r="L226" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="227" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M226" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A227" s="6" t="s">
         <v>632</v>
       </c>
@@ -44056,8 +44738,11 @@
       <c r="L227" s="13" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="228" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M227" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A228" s="6" t="s">
         <v>649</v>
       </c>
@@ -44092,8 +44777,11 @@
       <c r="L228" s="6" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="229" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M228" s="6" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A229" s="6" t="s">
         <v>649</v>
       </c>
@@ -44128,8 +44816,11 @@
       <c r="L229" s="6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="230" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M229" s="6" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A230" s="6" t="s">
         <v>649</v>
       </c>
@@ -44164,8 +44855,11 @@
       <c r="L230" s="6" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="231" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M230" s="6" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A231" s="6" t="s">
         <v>649</v>
       </c>
@@ -44200,8 +44894,11 @@
       <c r="L231" s="6" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="232" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M231" s="6" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A232" s="6" t="s">
         <v>649</v>
       </c>
@@ -44236,8 +44933,11 @@
       <c r="L232" s="6" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="233" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M232" s="6" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A233" s="6" t="s">
         <v>649</v>
       </c>
@@ -44272,8 +44972,11 @@
       <c r="L233" s="6" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="234" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M233" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A234" s="6" t="s">
         <v>649</v>
       </c>
@@ -44308,8 +45011,11 @@
       <c r="L234" s="6" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="235" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M234" s="6" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A235" s="6" t="s">
         <v>649</v>
       </c>
@@ -44344,8 +45050,11 @@
       <c r="L235" s="6" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="236" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M235" s="6" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A236" s="6" t="s">
         <v>649</v>
       </c>
@@ -44380,8 +45089,11 @@
       <c r="L236" s="6" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="237" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M236" s="6" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A237" s="6" t="s">
         <v>649</v>
       </c>
@@ -44416,8 +45128,11 @@
       <c r="L237" s="6" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="238" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M237" s="6" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A238" s="6" t="s">
         <v>649</v>
       </c>
@@ -44452,8 +45167,11 @@
       <c r="L238" s="6" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="239" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M238" s="6" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A239" s="6" t="s">
         <v>649</v>
       </c>
@@ -44488,8 +45206,11 @@
       <c r="L239" s="6" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="240" spans="1:12" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="M239" s="6" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" s="1" customFormat="1" ht="13" customHeight="1">
       <c r="A240" s="6" t="s">
         <v>649</v>
       </c>
@@ -44524,8 +45245,11 @@
       <c r="L240" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="241" spans="1:12" s="5" customFormat="1" ht="13" customHeight="1">
+      <c r="M240" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" s="5" customFormat="1" ht="13" customHeight="1">
       <c r="A241" s="2" t="s">
         <v>649</v>
       </c>
@@ -44560,8 +45284,11 @@
       <c r="L241" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="242" spans="1:12" ht="13" customHeight="1">
+      <c r="M241" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" ht="13" customHeight="1">
       <c r="A242" s="2" t="s">
         <v>671</v>
       </c>
@@ -44596,8 +45323,11 @@
       <c r="L242" s="3" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="243" spans="1:12" ht="13" customHeight="1">
+      <c r="M242" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" ht="13" customHeight="1">
       <c r="A243" s="2" t="s">
         <v>671</v>
       </c>
@@ -44632,8 +45362,11 @@
       <c r="L243" s="3" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="244" spans="1:12" ht="13" customHeight="1">
+      <c r="M243" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" ht="13" customHeight="1">
       <c r="A244" s="2" t="s">
         <v>671</v>
       </c>
@@ -44668,8 +45401,11 @@
       <c r="L244" s="3" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="245" spans="1:12" ht="13" customHeight="1">
+      <c r="M244" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" ht="13" customHeight="1">
       <c r="A245" s="2" t="s">
         <v>671</v>
       </c>
@@ -44704,8 +45440,11 @@
       <c r="L245" s="3" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="246" spans="1:12" ht="13" customHeight="1">
+      <c r="M245" s="3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" ht="13" customHeight="1">
       <c r="A246" s="2" t="s">
         <v>671</v>
       </c>
@@ -44740,8 +45479,11 @@
       <c r="L246" s="3" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" ht="13" customHeight="1">
+      <c r="M246" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" ht="13" customHeight="1">
       <c r="A247" s="2" t="s">
         <v>671</v>
       </c>
@@ -44776,8 +45518,11 @@
       <c r="L247" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="248" spans="1:12" ht="13" customHeight="1">
+      <c r="M247" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" ht="13" customHeight="1">
       <c r="A248" s="2" t="s">
         <v>671</v>
       </c>
@@ -44812,8 +45557,11 @@
       <c r="L248" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="249" spans="1:12" ht="13" customHeight="1">
+      <c r="M248" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" ht="13" customHeight="1">
       <c r="A249" s="2" t="s">
         <v>1270</v>
       </c>
@@ -44848,8 +45596,11 @@
       <c r="L249" s="3" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="250" spans="1:12" ht="13" customHeight="1">
+      <c r="M249" s="3" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" ht="13" customHeight="1">
       <c r="A250" s="2" t="s">
         <v>1270</v>
       </c>
@@ -44884,8 +45635,11 @@
       <c r="L250" s="3" t="s">
         <v>1272</v>
       </c>
-    </row>
-    <row r="251" spans="1:12" ht="13" customHeight="1">
+      <c r="M250" s="3" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" ht="13" customHeight="1">
       <c r="A251" s="2" t="s">
         <v>1270</v>
       </c>
@@ -44920,8 +45674,11 @@
       <c r="L251" s="3" t="s">
         <v>1273</v>
       </c>
-    </row>
-    <row r="252" spans="1:12" ht="13" customHeight="1">
+      <c r="M251" s="3" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" ht="13" customHeight="1">
       <c r="A252" s="2" t="s">
         <v>1270</v>
       </c>
@@ -44956,8 +45713,11 @@
       <c r="L252" s="3" t="s">
         <v>1274</v>
       </c>
-    </row>
-    <row r="253" spans="1:12" ht="13" customHeight="1">
+      <c r="M252" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" ht="13" customHeight="1">
       <c r="A253" s="2" t="s">
         <v>1270</v>
       </c>
@@ -44992,8 +45752,11 @@
       <c r="L253" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="254" spans="1:12" ht="13" customHeight="1">
+      <c r="M253" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" ht="13" customHeight="1">
       <c r="A254" s="2" t="s">
         <v>1265</v>
       </c>
@@ -45028,8 +45791,11 @@
       <c r="L254" s="3" t="s">
         <v>1266</v>
       </c>
-    </row>
-    <row r="255" spans="1:12" ht="13" customHeight="1">
+      <c r="M254" s="3" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" ht="13" customHeight="1">
       <c r="A255" s="2" t="s">
         <v>1265</v>
       </c>
@@ -45064,8 +45830,11 @@
       <c r="L255" s="3" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="256" spans="1:12" ht="13" customHeight="1">
+      <c r="M255" s="3" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" ht="13" customHeight="1">
       <c r="A256" s="2" t="s">
         <v>1265</v>
       </c>
@@ -45100,8 +45869,11 @@
       <c r="L256" s="3" t="s">
         <v>1268</v>
       </c>
-    </row>
-    <row r="257" spans="1:21" ht="13" customHeight="1">
+      <c r="M256" s="3" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="257" spans="1:22" ht="13" customHeight="1">
       <c r="A257" s="2" t="s">
         <v>1265</v>
       </c>
@@ -45136,8 +45908,11 @@
       <c r="L257" s="3" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="258" spans="1:21" ht="13" customHeight="1">
+      <c r="M257" s="3" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="258" spans="1:22" ht="13" customHeight="1">
       <c r="A258" s="2" t="s">
         <v>1265</v>
       </c>
@@ -45172,8 +45947,11 @@
       <c r="L258" s="13" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="259" spans="1:21" ht="13" customHeight="1">
+      <c r="M258" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="259" spans="1:22" ht="13" customHeight="1">
       <c r="A259" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45192,8 +45970,9 @@
       <c r="J259" s="13"/>
       <c r="K259" s="13"/>
       <c r="L259" s="13"/>
-    </row>
-    <row r="260" spans="1:21" ht="13" customHeight="1">
+      <c r="M259" s="13"/>
+    </row>
+    <row r="260" spans="1:22" ht="13" customHeight="1">
       <c r="A260" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45212,8 +45991,9 @@
       <c r="J260" s="13"/>
       <c r="K260" s="13"/>
       <c r="L260" s="13"/>
-    </row>
-    <row r="261" spans="1:21" ht="13" customHeight="1">
+      <c r="M260" s="13"/>
+    </row>
+    <row r="261" spans="1:22" ht="13" customHeight="1">
       <c r="A261" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45232,8 +46012,9 @@
       <c r="J261" s="13"/>
       <c r="K261" s="13"/>
       <c r="L261" s="13"/>
-    </row>
-    <row r="262" spans="1:21" ht="13" customHeight="1">
+      <c r="M261" s="13"/>
+    </row>
+    <row r="262" spans="1:22" ht="13" customHeight="1">
       <c r="A262" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45252,8 +46033,9 @@
       <c r="J262" s="13"/>
       <c r="K262" s="13"/>
       <c r="L262" s="13"/>
-    </row>
-    <row r="263" spans="1:21" ht="13" customHeight="1">
+      <c r="M262" s="13"/>
+    </row>
+    <row r="263" spans="1:22" ht="13" customHeight="1">
       <c r="A263" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45272,8 +46054,9 @@
       <c r="J263" s="13"/>
       <c r="K263" s="13"/>
       <c r="L263" s="13"/>
-    </row>
-    <row r="264" spans="1:21" ht="13" customHeight="1">
+      <c r="M263" s="13"/>
+    </row>
+    <row r="264" spans="1:22" ht="13" customHeight="1">
       <c r="A264" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45292,8 +46075,9 @@
       <c r="J264" s="13"/>
       <c r="K264" s="13"/>
       <c r="L264" s="13"/>
-    </row>
-    <row r="265" spans="1:21" ht="13" customHeight="1">
+      <c r="M264" s="13"/>
+    </row>
+    <row r="265" spans="1:22" ht="13" customHeight="1">
       <c r="A265" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45312,8 +46096,9 @@
       <c r="J265" s="13"/>
       <c r="K265" s="13"/>
       <c r="L265" s="13"/>
-    </row>
-    <row r="266" spans="1:21" ht="13" customHeight="1">
+      <c r="M265" s="13"/>
+    </row>
+    <row r="266" spans="1:22" ht="13" customHeight="1">
       <c r="A266" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45332,8 +46117,9 @@
       <c r="J266" s="13"/>
       <c r="K266" s="13"/>
       <c r="L266" s="13"/>
-    </row>
-    <row r="267" spans="1:21" ht="13" customHeight="1">
+      <c r="M266" s="13"/>
+    </row>
+    <row r="267" spans="1:22" ht="13" customHeight="1">
       <c r="A267" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45352,8 +46138,9 @@
       <c r="J267" s="13"/>
       <c r="K267" s="13"/>
       <c r="L267" s="13"/>
-    </row>
-    <row r="268" spans="1:21" ht="13" customHeight="1">
+      <c r="M267" s="13"/>
+    </row>
+    <row r="268" spans="1:22" ht="13" customHeight="1">
       <c r="A268" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45372,8 +46159,9 @@
       <c r="J268" s="13"/>
       <c r="K268" s="13"/>
       <c r="L268" s="13"/>
-    </row>
-    <row r="269" spans="1:21" ht="13" customHeight="1">
+      <c r="M268" s="13"/>
+    </row>
+    <row r="269" spans="1:22" ht="13" customHeight="1">
       <c r="A269" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45392,8 +46180,9 @@
       <c r="J269" s="13"/>
       <c r="K269" s="13"/>
       <c r="L269" s="13"/>
-    </row>
-    <row r="270" spans="1:21" ht="13" customHeight="1">
+      <c r="M269" s="13"/>
+    </row>
+    <row r="270" spans="1:22" ht="13" customHeight="1">
       <c r="A270" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45412,8 +46201,9 @@
       <c r="J270" s="13"/>
       <c r="K270" s="13"/>
       <c r="L270" s="13"/>
-    </row>
-    <row r="271" spans="1:21" ht="13" customHeight="1">
+      <c r="M270" s="13"/>
+    </row>
+    <row r="271" spans="1:22" ht="13" customHeight="1">
       <c r="A271" s="13" t="s">
         <v>2291</v>
       </c>
@@ -45432,8 +46222,9 @@
       <c r="J271" s="13"/>
       <c r="K271" s="13"/>
       <c r="L271" s="13"/>
-    </row>
-    <row r="272" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="M271" s="13"/>
+    </row>
+    <row r="272" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A272" s="29" t="s">
         <v>979</v>
       </c>
@@ -45468,7 +46259,9 @@
       <c r="L272" s="29" t="s">
         <v>1084</v>
       </c>
-      <c r="M272" s="34"/>
+      <c r="M272" s="29" t="s">
+        <v>1084</v>
+      </c>
       <c r="N272" s="34"/>
       <c r="O272" s="34"/>
       <c r="P272" s="34"/>
@@ -45477,8 +46270,9 @@
       <c r="S272" s="34"/>
       <c r="T272" s="34"/>
       <c r="U272" s="34"/>
-    </row>
-    <row r="273" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V272" s="34"/>
+    </row>
+    <row r="273" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A273" s="29" t="s">
         <v>979</v>
       </c>
@@ -45513,7 +46307,9 @@
       <c r="L273" s="29" t="s">
         <v>1215</v>
       </c>
-      <c r="M273" s="34"/>
+      <c r="M273" s="29" t="s">
+        <v>1215</v>
+      </c>
       <c r="N273" s="34"/>
       <c r="O273" s="34"/>
       <c r="P273" s="34"/>
@@ -45522,8 +46318,9 @@
       <c r="S273" s="34"/>
       <c r="T273" s="34"/>
       <c r="U273" s="34"/>
-    </row>
-    <row r="274" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V273" s="34"/>
+    </row>
+    <row r="274" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A274" s="29" t="s">
         <v>979</v>
       </c>
@@ -45558,7 +46355,9 @@
       <c r="L274" s="56" t="s">
         <v>1156</v>
       </c>
-      <c r="M274" s="34"/>
+      <c r="M274" s="56" t="s">
+        <v>1156</v>
+      </c>
       <c r="N274" s="34"/>
       <c r="O274" s="34"/>
       <c r="P274" s="34"/>
@@ -45567,8 +46366,9 @@
       <c r="S274" s="34"/>
       <c r="T274" s="34"/>
       <c r="U274" s="34"/>
-    </row>
-    <row r="275" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V274" s="34"/>
+    </row>
+    <row r="275" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A275" s="29" t="s">
         <v>979</v>
       </c>
@@ -45603,7 +46403,9 @@
       <c r="L275" s="56" t="s">
         <v>1158</v>
       </c>
-      <c r="M275" s="34"/>
+      <c r="M275" s="56" t="s">
+        <v>1158</v>
+      </c>
       <c r="N275" s="34"/>
       <c r="O275" s="34"/>
       <c r="P275" s="34"/>
@@ -45612,8 +46414,9 @@
       <c r="S275" s="34"/>
       <c r="T275" s="34"/>
       <c r="U275" s="34"/>
-    </row>
-    <row r="276" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V275" s="34"/>
+    </row>
+    <row r="276" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A276" s="29" t="s">
         <v>979</v>
       </c>
@@ -45648,7 +46451,9 @@
       <c r="L276" s="56" t="s">
         <v>1217</v>
       </c>
-      <c r="M276" s="34"/>
+      <c r="M276" s="56" t="s">
+        <v>1217</v>
+      </c>
       <c r="N276" s="34"/>
       <c r="O276" s="34"/>
       <c r="P276" s="34"/>
@@ -45657,8 +46462,9 @@
       <c r="S276" s="34"/>
       <c r="T276" s="34"/>
       <c r="U276" s="34"/>
-    </row>
-    <row r="277" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V276" s="34"/>
+    </row>
+    <row r="277" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A277" s="29" t="s">
         <v>979</v>
       </c>
@@ -45693,7 +46499,9 @@
       <c r="L277" s="56" t="s">
         <v>1160</v>
       </c>
-      <c r="M277" s="34"/>
+      <c r="M277" s="56" t="s">
+        <v>1160</v>
+      </c>
       <c r="N277" s="34"/>
       <c r="O277" s="34"/>
       <c r="P277" s="34"/>
@@ -45702,8 +46510,9 @@
       <c r="S277" s="34"/>
       <c r="T277" s="34"/>
       <c r="U277" s="34"/>
-    </row>
-    <row r="278" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V277" s="34"/>
+    </row>
+    <row r="278" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A278" s="29" t="s">
         <v>979</v>
       </c>
@@ -45738,7 +46547,9 @@
       <c r="L278" s="56" t="s">
         <v>1162</v>
       </c>
-      <c r="M278" s="34"/>
+      <c r="M278" s="56" t="s">
+        <v>1162</v>
+      </c>
       <c r="N278" s="34"/>
       <c r="O278" s="34"/>
       <c r="P278" s="34"/>
@@ -45747,8 +46558,9 @@
       <c r="S278" s="34"/>
       <c r="T278" s="34"/>
       <c r="U278" s="34"/>
-    </row>
-    <row r="279" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V278" s="34"/>
+    </row>
+    <row r="279" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A279" s="29" t="s">
         <v>979</v>
       </c>
@@ -45783,7 +46595,9 @@
       <c r="L279" s="56" t="s">
         <v>1164</v>
       </c>
-      <c r="M279" s="34"/>
+      <c r="M279" s="56" t="s">
+        <v>1164</v>
+      </c>
       <c r="N279" s="34"/>
       <c r="O279" s="34"/>
       <c r="P279" s="34"/>
@@ -45792,8 +46606,9 @@
       <c r="S279" s="34"/>
       <c r="T279" s="34"/>
       <c r="U279" s="34"/>
-    </row>
-    <row r="280" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V279" s="34"/>
+    </row>
+    <row r="280" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A280" s="29" t="s">
         <v>979</v>
       </c>
@@ -45828,7 +46643,9 @@
       <c r="L280" s="56" t="s">
         <v>1166</v>
       </c>
-      <c r="M280" s="34"/>
+      <c r="M280" s="56" t="s">
+        <v>1166</v>
+      </c>
       <c r="N280" s="34"/>
       <c r="O280" s="34"/>
       <c r="P280" s="34"/>
@@ -45837,8 +46654,9 @@
       <c r="S280" s="34"/>
       <c r="T280" s="34"/>
       <c r="U280" s="34"/>
-    </row>
-    <row r="281" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
+      <c r="V280" s="34"/>
+    </row>
+    <row r="281" spans="1:22" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A281" s="29" t="s">
         <v>979</v>
       </c>
@@ -45873,7 +46691,9 @@
       <c r="L281" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="M281" s="34"/>
+      <c r="M281" s="13" t="s">
+        <v>446</v>
+      </c>
       <c r="N281" s="34"/>
       <c r="O281" s="34"/>
       <c r="P281" s="34"/>
@@ -45882,6 +46702,7 @@
       <c r="S281" s="34"/>
       <c r="T281" s="34"/>
       <c r="U281" s="34"/>
+      <c r="V281" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45922,7 +46743,7 @@
         <v>599</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>602</v>
@@ -45945,7 +46766,7 @@
         <v>1084</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="E2" s="18" t="b">
         <v>1</v>

</xml_diff>